<commit_message>
Write File 06 june
</commit_message>
<xml_diff>
--- a/resources/testdata/Testdata.xlsx
+++ b/resources/testdata/Testdata.xlsx
@@ -1,145 +1,53 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Credentials" sheetId="1" r:id="rId1"/>
-    <sheet name="Address" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Credentials" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Address" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" concurrentCalc="0"/>
+  <definedNames/>
+  <calcPr calcId="122211" fullCalcOnLoad="1" concurrentCalc="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>knagesh143s@gmail.com</t>
-  </si>
-  <si>
-    <t>knagesh143s</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Street</t>
-  </si>
-  <si>
-    <t>Secondary Address</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>ZipCode</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Website</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Interest</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>BirthDate</t>
-  </si>
-  <si>
-    <t>Nagesh</t>
-  </si>
-  <si>
-    <t>Kadam</t>
-  </si>
-  <si>
-    <t>Datta Mandir Road</t>
-  </si>
-  <si>
-    <t>Wanjarkheda</t>
-  </si>
-  <si>
-    <t>Tq &amp; Dist:-Latur</t>
-  </si>
-  <si>
-    <t>GA</t>
-  </si>
-  <si>
-    <t>United State</t>
-  </si>
-  <si>
-    <t>413 511</t>
-  </si>
-  <si>
-    <t>http://a.testaddressbook.com/addresses/new</t>
-  </si>
-  <si>
-    <t>Climb</t>
-  </si>
-  <si>
-    <t>Notes Added</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d/mmm/yy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="12"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -162,26 +70,20 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -471,33 +373,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col width="23.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="12.140625" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Username</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Password</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>knagesh143s@gmail.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>knagesh143s</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -506,117 +420,193 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col width="11.42578125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="11.140625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="17.5703125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="19.85546875" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="14.7109375" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="6.140625" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="12" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="8.85546875" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="4.7109375" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="44.5703125" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="11" bestFit="1" customWidth="1" min="11" max="11"/>
+    <col width="8.5703125" bestFit="1" customWidth="1" min="12" max="12"/>
+    <col width="12.5703125" bestFit="1" customWidth="1" min="13" max="13"/>
+    <col width="10.42578125" bestFit="1" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>17</v>
+    <row r="1" ht="15.75" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Street</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Secondary Address</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>State</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ZipCode</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Website</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Phone</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Interest</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>BirthDate</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="2">
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Nagesh</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Kadam</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>Datta Mandir Road</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Wanjarkheda</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>Tq &amp; Dist:-Latur</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>United State</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>413 511</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="2">
+      <c r="J2" s="3" t="inlineStr">
+        <is>
+          <t>http://a.testaddressbook.com/addresses/new</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="n">
         <v>1234567890</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="4">
+      <c r="L2" s="2" t="inlineStr">
+        <is>
+          <t>Climb</t>
+        </is>
+      </c>
+      <c r="M2" s="2" t="inlineStr">
+        <is>
+          <t>Notes Added</t>
+        </is>
+      </c>
+      <c r="N2" s="4" t="n">
         <v>32663</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Nagesh</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Kadam</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Tq &amp; Dist:-Latur</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -628,12 +618,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>